<commit_message>
casi listo parte 2
</commit_message>
<xml_diff>
--- a/2daParte/Mediciones_AmplificadorEC.xlsx
+++ b/2daParte/Mediciones_AmplificadorEC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D488EB72-D84B-480E-9D1D-2EB3CDDEF383}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B116E5D-25E5-4284-B21E-C4DB98C208B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
         <v>9.1000000000000004E-3</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" ref="H5:H24" si="0">10000*G5/(F5-G5)</f>
+        <f t="shared" ref="H5:H23" si="0">10000*G5/(F5-G5)</f>
         <v>7520.6611570247933</v>
       </c>
       <c r="I5" s="2"/>
@@ -577,7 +577,7 @@
         <v>3.4</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" ref="L5:L24" si="1">-(J5-K5)*10000/K5</f>
+        <f t="shared" ref="L5:L23" si="1">-(J5-K5)*10000/K5</f>
         <v>7794.1176470588234</v>
       </c>
       <c r="M5" s="2"/>
@@ -1211,6 +1211,17 @@
         <v>5315.78947368421</v>
       </c>
       <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>100000</v>
+      </c>
+      <c r="C24" s="5">
+        <v>38.9</v>
+      </c>
+      <c r="D24" s="5">
+        <v>180</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>

</xml_diff>